<commit_message>
Mise à jour du diagramme des classes
</commit_message>
<xml_diff>
--- a/Cahier des charges + analyse/journal + estimatif.xlsx
+++ b/Cahier des charges + analyse/journal + estimatif.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Liste des tâches</t>
   </si>
@@ -124,6 +124,12 @@
     <t>Modification du schema UML + schema base de donnée:
 Rajout d'une playlist par défaut dans la classe Exercice
 Rajout d'une table playlist pour lier un morceau à un Exercice ou un ElementSequence</t>
+  </si>
+  <si>
+    <t>Création et début d'implémentation de la classe DAOBase gérant les entrées sorties vers la base de donnée</t>
+  </si>
+  <si>
+    <t>Mise à jour du diagramme des classes suite aux modifications apportées</t>
   </si>
 </sst>
 </file>
@@ -863,41 +869,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -908,12 +885,41 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1819,7 +1825,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1836,18 +1842,18 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="59" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1">
-      <c r="A4" s="69">
+      <c r="A4" s="60">
         <v>42019</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1858,7 +1864,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="70"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
@@ -1867,7 +1873,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="71"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
@@ -1876,7 +1882,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1">
-      <c r="A7" s="69">
+      <c r="A7" s="60">
         <v>42039</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1887,7 +1893,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="71"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
@@ -1896,7 +1902,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1">
-      <c r="A9" s="69">
+      <c r="A9" s="60">
         <v>42043</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1907,7 +1913,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A10" s="71"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="8" t="s">
         <v>2</v>
       </c>
@@ -1916,7 +1922,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1">
-      <c r="A11" s="69">
+      <c r="A11" s="60">
         <v>42046</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1927,7 +1933,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A12" s="71"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
@@ -1936,7 +1942,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A13" s="69">
+      <c r="A13" s="60">
         <v>42049</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1947,7 +1953,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A14" s="71"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="8" t="s">
         <v>2</v>
       </c>
@@ -1955,15 +1961,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="1" customFormat="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="14"/>
-    </row>
-    <row r="16" spans="1:3" s="1" customFormat="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="14"/>
+    <row r="15" spans="1:3" s="1" customFormat="1" ht="30">
+      <c r="A15" s="60">
+        <v>42052</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A16" s="62"/>
+      <c r="B16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:3" s="1" customFormat="1">
       <c r="A17" s="13"/>
@@ -2006,7 +2022,8 @@
       <c r="C24" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
@@ -2046,10 +2063,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="58"/>
+      <c r="B2" s="64"/>
       <c r="C2" s="49" t="s">
         <v>1</v>
       </c>
@@ -2058,8 +2075,8 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="51" t="s">
         <v>3</v>
       </c>
@@ -2068,8 +2085,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="51" t="s">
         <v>2</v>
       </c>
@@ -2078,8 +2095,8 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="51" t="s">
         <v>26</v>
       </c>
@@ -2088,8 +2105,8 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="51" t="s">
         <v>25</v>
       </c>
@@ -2098,8 +2115,8 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="61"/>
-      <c r="B7" s="62"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="51" t="s">
         <v>17</v>
       </c>
@@ -2108,10 +2125,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="72" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="53" t="s">
@@ -2122,8 +2139,8 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="64"/>
-      <c r="B9" s="67"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="53" t="s">
         <v>7</v>
       </c>
@@ -2132,8 +2149,8 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="64"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="53" t="s">
         <v>9</v>
       </c>
@@ -2142,8 +2159,8 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="64"/>
-      <c r="B11" s="67"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="53" t="s">
         <v>11</v>
       </c>
@@ -2152,8 +2169,8 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="64"/>
-      <c r="B12" s="67"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="53" t="s">
         <v>10</v>
       </c>
@@ -2162,8 +2179,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A13" s="65"/>
-      <c r="B13" s="68"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="55" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Mise a jour diagramme des classes
nouvelle classe Morceau + nouvelles fonctions
</commit_message>
<xml_diff>
--- a/Cahier des charges + analyse/journal + estimatif.xlsx
+++ b/Cahier des charges + analyse/journal + estimatif.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>Liste des tâches</t>
   </si>
@@ -130,6 +130,20 @@
   </si>
   <si>
     <t>Mise à jour du diagramme des classes suite aux modifications apportées</t>
+  </si>
+  <si>
+    <t>Modification du schema UML + schema base de donnée:
+Rajout de la classe Morceau
+remplacement des Uri par les id des morceaux depuis la base de donnée interne du téléphone
+Ajout d'un champ JouerPlaylist dans la table ElementSequence</t>
+  </si>
+  <si>
+    <t>Creation de la classe morceau + implémentation des getter et setter</t>
+  </si>
+  <si>
+    <t>travail sur DAOBase : 
+saveLibrairieExercice/restoreLibrairieExercice
+restoreLibrairieSequence</t>
   </si>
 </sst>
 </file>
@@ -879,10 +893,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1825,7 +1839,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1864,7 +1878,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="61"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
@@ -1873,7 +1887,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="62"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
@@ -1893,7 +1907,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="62"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
@@ -1913,7 +1927,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A10" s="62"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="8" t="s">
         <v>2</v>
       </c>
@@ -1933,7 +1947,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A12" s="62"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
@@ -1953,7 +1967,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A14" s="62"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="8" t="s">
         <v>2</v>
       </c>
@@ -1973,7 +1987,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A16" s="62"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="8" t="s">
         <v>2</v>
       </c>
@@ -1981,20 +1995,34 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="1" customFormat="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="14"/>
+    <row r="17" spans="1:3" s="1" customFormat="1" ht="60">
+      <c r="A17" s="60">
+        <v>42053</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="14"/>
-    </row>
-    <row r="19" spans="1:3" s="1" customFormat="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="14"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
+      <c r="A19" s="61"/>
+      <c r="B19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1">
       <c r="A20" s="13"/>
@@ -2022,7 +2050,8 @@
       <c r="C24" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>

</xml_diff>

<commit_message>
Maj diagramme de classe : ChronoService
</commit_message>
<xml_diff>
--- a/Cahier des charges + analyse/journal + estimatif.xlsx
+++ b/Cahier des charges + analyse/journal + estimatif.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>Liste des tâches</t>
   </si>
@@ -132,18 +132,31 @@
     <t>Mise à jour du diagramme des classes suite aux modifications apportées</t>
   </si>
   <si>
-    <t>Modification du schema UML + schema base de donnée:
+    <t>Creation de la classe morceau + implémentation des getter et setter</t>
+  </si>
+  <si>
+    <t>travail sur DAOBase : 
+saveLibrairieExercice/restoreLibrairieExercice
+restoreLibrairieSequence</t>
+  </si>
+  <si>
+    <t>Création de ChronoService et des classes tierse 
+implémentation du chronometre dans ChronoService</t>
+  </si>
+  <si>
+    <t>Implémentation de l'interface de ChronometreActivity</t>
+  </si>
+  <si>
+    <t>Création et utilisation des services et de la classe CountDownTimer</t>
+  </si>
+  <si>
+    <t>Modification du diagramme de classe  + schema base de donnée:
 Rajout de la classe Morceau
 remplacement des Uri par les id des morceaux depuis la base de donnée interne du téléphone
 Ajout d'un champ JouerPlaylist dans la table ElementSequence</t>
   </si>
   <si>
-    <t>Creation de la classe morceau + implémentation des getter et setter</t>
-  </si>
-  <si>
-    <t>travail sur DAOBase : 
-saveLibrairieExercice/restoreLibrairieExercice
-restoreLibrairieSequence</t>
+    <t>Diagramme de classe : ChronoService + classes annexes</t>
   </si>
 </sst>
 </file>
@@ -214,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -729,11 +742,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -893,47 +919,53 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1836,10 +1868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1878,7 +1910,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="62"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
@@ -1887,7 +1919,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="61"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
@@ -1907,7 +1939,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="61"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
@@ -1927,7 +1959,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A10" s="61"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="8" t="s">
         <v>2</v>
       </c>
@@ -1947,7 +1979,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A12" s="61"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="8" t="s">
         <v>2</v>
       </c>
@@ -1967,7 +1999,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A14" s="61"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="8" t="s">
         <v>2</v>
       </c>
@@ -1987,7 +2019,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A16" s="61"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="8" t="s">
         <v>2</v>
       </c>
@@ -2003,54 +2035,78 @@
         <v>2</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1">
-      <c r="A18" s="62"/>
+      <c r="A18" s="61"/>
       <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A19" s="61"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="1" customFormat="1" ht="30">
+      <c r="A20" s="60">
+        <v>42058</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="1" customFormat="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="14"/>
-    </row>
     <row r="21" spans="1:3" s="1" customFormat="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="14"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1">
-      <c r="A22" s="13"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="14"/>
-    </row>
-    <row r="23" spans="1:3" s="1" customFormat="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="14"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A23" s="62"/>
+      <c r="B23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1">
       <c r="A24" s="13"/>
       <c r="B24" s="3"/>
       <c r="C24" s="14"/>
     </row>
+    <row r="25" spans="1:3" s="1" customFormat="1">
+      <c r="A25" s="13"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A4:A6"/>

</xml_diff>

<commit_message>
cahier des charges + présentation
</commit_message>
<xml_diff>
--- a/Cahier des charges + analyse/journal + estimatif.xlsx
+++ b/Cahier des charges + analyse/journal + estimatif.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="21315" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="21315" windowHeight="8265" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plannification" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
   <si>
     <t>Liste des tâches</t>
   </si>
@@ -163,6 +163,24 @@
   </si>
   <si>
     <t xml:space="preserve">ChronometreActivity : Gestion du click et de la position affichée dans la ListView </t>
+  </si>
+  <si>
+    <t>Ios</t>
+  </si>
+  <si>
+    <t>Documentation projet</t>
+  </si>
+  <si>
+    <t>Rédaction du dossier de projet</t>
+  </si>
+  <si>
+    <t>Windows phone</t>
+  </si>
+  <si>
+    <t>Multimédia</t>
+  </si>
+  <si>
+    <t>Synthèse vocale</t>
   </si>
 </sst>
 </file>
@@ -172,17 +190,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-yy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +243,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="41">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -346,15 +381,6 @@
     </border>
     <border>
       <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thick">
@@ -377,7 +403,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thick">
@@ -395,21 +421,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -423,66 +434,10 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -761,11 +716,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -800,170 +840,198 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1263,22 +1331,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD18"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="A4:D17"/>
+      <selection activeCell="A4" sqref="A4:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="45" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
     <col min="6" max="30" width="3.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1299,115 +1368,116 @@
       <c r="X1" s="11"/>
       <c r="Y1" s="11"/>
     </row>
-    <row r="3" spans="1:30" ht="20.25" customHeight="1" thickBot="1"/>
-    <row r="4" spans="1:30" ht="72.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="39" t="s">
+    <row r="3" spans="1:31" ht="20.25" customHeight="1"/>
+    <row r="4" spans="1:31" ht="72.75" customHeight="1">
+      <c r="A4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="9">
         <v>1</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="9">
         <v>2</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="9">
         <v>3</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="9">
         <v>4</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="9">
         <v>5</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="9">
         <v>6</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="9">
         <v>7</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="9">
         <v>8</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="9">
         <v>9</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="9">
         <v>10</v>
       </c>
-      <c r="P4" s="24">
+      <c r="P4" s="9">
         <v>11</v>
       </c>
-      <c r="Q4" s="24">
+      <c r="Q4" s="9">
         <v>12</v>
       </c>
-      <c r="R4" s="24">
+      <c r="R4" s="9">
         <v>13</v>
       </c>
-      <c r="S4" s="24">
+      <c r="S4" s="9">
         <v>14</v>
       </c>
-      <c r="T4" s="24">
+      <c r="T4" s="9">
         <v>15</v>
       </c>
-      <c r="U4" s="24">
+      <c r="U4" s="9">
         <v>16</v>
       </c>
-      <c r="V4" s="24">
+      <c r="V4" s="9">
         <v>17</v>
       </c>
-      <c r="W4" s="24">
+      <c r="W4" s="9">
         <v>18</v>
       </c>
-      <c r="X4" s="24">
+      <c r="X4" s="9">
         <v>19</v>
       </c>
-      <c r="Y4" s="24">
+      <c r="Y4" s="9">
         <v>20</v>
       </c>
-      <c r="Z4" s="24">
+      <c r="Z4" s="9">
         <v>21</v>
       </c>
-      <c r="AA4" s="24">
+      <c r="AA4" s="9">
         <v>22</v>
       </c>
-      <c r="AB4" s="24">
+      <c r="AB4" s="9">
         <v>23</v>
       </c>
-      <c r="AC4" s="24">
+      <c r="AC4" s="9">
         <v>24</v>
       </c>
-      <c r="AD4" s="25">
+      <c r="AD4" s="9">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" ht="16.5" thickTop="1">
-      <c r="A5" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="29">
-        <v>5</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="AE4" s="49"/>
+    </row>
+    <row r="5" spans="1:31" ht="15.75">
+      <c r="A5" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
@@ -1422,26 +1492,27 @@
       <c r="AA5" s="9"/>
       <c r="AB5" s="9"/>
       <c r="AC5" s="9"/>
-      <c r="AD5" s="12"/>
-    </row>
-    <row r="6" spans="1:30">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="33">
-        <v>5</v>
-      </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="49"/>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="49"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
@@ -1458,28 +1529,29 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
       <c r="AC6" s="9"/>
-      <c r="AD6" s="12"/>
-    </row>
-    <row r="7" spans="1:30">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="33">
-        <v>6</v>
-      </c>
-      <c r="E7" s="31"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="49"/>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="9">
+        <v>4</v>
+      </c>
+      <c r="E7" s="49"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
@@ -1494,23 +1566,26 @@
       <c r="AA7" s="9"/>
       <c r="AB7" s="9"/>
       <c r="AC7" s="9"/>
-      <c r="AD7" s="12"/>
-    </row>
-    <row r="8" spans="1:30">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="33">
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="49"/>
+    </row>
+    <row r="8" spans="1:31" ht="15.75">
+      <c r="A8" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="D8" s="9">
+        <v>5</v>
+      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
@@ -1530,28 +1605,29 @@
       <c r="AA8" s="9"/>
       <c r="AB8" s="9"/>
       <c r="AC8" s="9"/>
-      <c r="AD8" s="12"/>
-    </row>
-    <row r="9" spans="1:30">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="33">
-        <v>4</v>
-      </c>
-      <c r="E9" s="31"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="49"/>
+    </row>
+    <row r="9" spans="1:31">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="9">
+        <v>5</v>
+      </c>
+      <c r="E9" s="49"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
@@ -1566,27 +1642,28 @@
       <c r="AA9" s="9"/>
       <c r="AB9" s="9"/>
       <c r="AC9" s="9"/>
-      <c r="AD9" s="12"/>
-    </row>
-    <row r="10" spans="1:30">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="33">
-        <v>4</v>
-      </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="49"/>
+    </row>
+    <row r="10" spans="1:31">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9">
+        <v>6</v>
+      </c>
+      <c r="E10" s="49"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
@@ -1602,19 +1679,24 @@
       <c r="AA10" s="9"/>
       <c r="AB10" s="9"/>
       <c r="AC10" s="9"/>
-      <c r="AD10" s="12"/>
-    </row>
-    <row r="11" spans="1:30">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="49"/>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="A11" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="9">
+        <v>6</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
@@ -1623,41 +1705,42 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
+      <c r="S11" s="15"/>
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
       <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
+      <c r="W11" s="15"/>
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
-      <c r="AD11" s="12"/>
-    </row>
-    <row r="12" spans="1:30" ht="15.75">
-      <c r="A12" s="34" t="s">
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="49"/>
+    </row>
+    <row r="12" spans="1:31" ht="15.75">
+      <c r="A12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -1674,18 +1757,19 @@
       <c r="AA12" s="9"/>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
-      <c r="AD12" s="12"/>
-    </row>
-    <row r="13" spans="1:30">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32" t="s">
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="49"/>
+    </row>
+    <row r="13" spans="1:31">
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="33">
-        <v>2</v>
-      </c>
-      <c r="E13" s="31"/>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="49"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -1694,8 +1778,8 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="9"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
@@ -1710,18 +1794,19 @@
       <c r="AA13" s="9"/>
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
-      <c r="AD13" s="12"/>
-    </row>
-    <row r="14" spans="1:30">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="33">
-        <v>1</v>
-      </c>
-      <c r="E14" s="31"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="49"/>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="49"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -1731,8 +1816,8 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="16"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
@@ -1746,18 +1831,19 @@
       <c r="AA14" s="9"/>
       <c r="AB14" s="9"/>
       <c r="AC14" s="9"/>
-      <c r="AD14" s="12"/>
-    </row>
-    <row r="15" spans="1:30">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="33">
-        <v>1</v>
-      </c>
-      <c r="E15" s="31"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="49"/>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="49"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -1767,8 +1853,8 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="13"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
@@ -1782,18 +1868,19 @@
       <c r="AA15" s="9"/>
       <c r="AB15" s="9"/>
       <c r="AC15" s="9"/>
-      <c r="AD15" s="12"/>
-    </row>
-    <row r="16" spans="1:30">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32" t="s">
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="49"/>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="33">
-        <v>2</v>
-      </c>
-      <c r="E16" s="31"/>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="49"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -1804,9 +1891,9 @@
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
       <c r="S16" s="9"/>
       <c r="T16" s="9"/>
       <c r="U16" s="9"/>
@@ -1818,45 +1905,416 @@
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
       <c r="AC16" s="9"/>
-      <c r="AD16" s="12"/>
-    </row>
-    <row r="17" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37" t="s">
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="49"/>
+    </row>
+    <row r="17" spans="1:31">
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="38">
-        <v>3</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20"/>
-      <c r="U17" s="20"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="19"/>
-      <c r="X17" s="19"/>
-      <c r="Y17" s="19"/>
-      <c r="Z17" s="19"/>
-      <c r="AA17" s="19"/>
-      <c r="AB17" s="19"/>
-      <c r="AC17" s="19"/>
-      <c r="AD17" s="22"/>
-    </row>
-    <row r="18" spans="1:30" ht="15.75" thickTop="1"/>
+      <c r="D17" s="9">
+        <v>2</v>
+      </c>
+      <c r="E17" s="49"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="49"/>
+      <c r="AD17" s="49"/>
+      <c r="AE17" s="49"/>
+    </row>
+    <row r="18" spans="1:31">
+      <c r="A18" s="49"/>
+      <c r="B18" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="9">
+        <v>2</v>
+      </c>
+      <c r="E18" s="49"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="49"/>
+      <c r="AD18" s="49"/>
+      <c r="AE18" s="49"/>
+    </row>
+    <row r="19" spans="1:31">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1</v>
+      </c>
+      <c r="E19" s="49"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="49"/>
+      <c r="AC19" s="49"/>
+      <c r="AD19" s="49"/>
+      <c r="AE19" s="49"/>
+    </row>
+    <row r="20" spans="1:31">
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="49"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="49"/>
+      <c r="AC20" s="49"/>
+      <c r="AD20" s="49"/>
+      <c r="AE20" s="49"/>
+    </row>
+    <row r="21" spans="1:31">
+      <c r="A21" s="49"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="49"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="49"/>
+      <c r="AB21" s="49"/>
+      <c r="AC21" s="49"/>
+      <c r="AD21" s="49"/>
+      <c r="AE21" s="49"/>
+    </row>
+    <row r="22" spans="1:31">
+      <c r="A22" s="49"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="E22" s="49"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="49"/>
+      <c r="AB22" s="49"/>
+      <c r="AC22" s="49"/>
+      <c r="AD22" s="49"/>
+      <c r="AE22" s="49"/>
+    </row>
+    <row r="23" spans="1:31">
+      <c r="A23" s="49"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="9">
+        <v>2</v>
+      </c>
+      <c r="E23" s="49"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="49"/>
+      <c r="AB23" s="49"/>
+      <c r="AC23" s="49"/>
+      <c r="AD23" s="49"/>
+      <c r="AE23" s="49"/>
+    </row>
+    <row r="24" spans="1:31">
+      <c r="A24" s="49"/>
+      <c r="B24" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="9">
+        <v>1</v>
+      </c>
+      <c r="E24" s="49"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="12"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="49"/>
+    </row>
+    <row r="25" spans="1:31">
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1</v>
+      </c>
+      <c r="E25" s="49"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="49"/>
+    </row>
+    <row r="26" spans="1:31">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1</v>
+      </c>
+      <c r="E26" s="49"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="15"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="49"/>
+    </row>
+    <row r="27" spans="1:31">
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="9"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="49"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1867,36 +2325,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11" style="72" customWidth="1"/>
+    <col min="1" max="1" width="11" style="32" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" style="9" customWidth="1"/>
     <col min="3" max="3" width="89.5703125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="29" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1">
-      <c r="A4" s="57">
+      <c r="A4" s="34">
         <v>42019</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1907,7 +2365,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="58"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -1916,7 +2374,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="59"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
@@ -1925,7 +2383,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1">
-      <c r="A7" s="57">
+      <c r="A7" s="34">
         <v>42039</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1936,7 +2394,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="59"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
@@ -1945,7 +2403,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1">
-      <c r="A9" s="57">
+      <c r="A9" s="34">
         <v>42043</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1956,7 +2414,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A10" s="59"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1965,7 +2423,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1">
-      <c r="A11" s="57">
+      <c r="A11" s="34">
         <v>42046</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1976,7 +2434,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A12" s="59"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="7" t="s">
         <v>2</v>
       </c>
@@ -1985,7 +2443,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A13" s="57">
+      <c r="A13" s="34">
         <v>42049</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1996,7 +2454,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A14" s="59"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="7" t="s">
         <v>2</v>
       </c>
@@ -2005,7 +2463,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A15" s="57">
+      <c r="A15" s="34">
         <v>42052</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2016,7 +2474,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A16" s="59"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
@@ -2025,7 +2483,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" s="1" customFormat="1" ht="60">
-      <c r="A17" s="57">
+      <c r="A17" s="34">
         <v>42053</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2036,7 +2494,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1">
-      <c r="A18" s="58"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
@@ -2045,7 +2503,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A19" s="59"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
@@ -2054,7 +2512,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A20" s="57">
+      <c r="A20" s="34">
         <v>42058</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -2065,16 +2523,16 @@
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1">
-      <c r="A21" s="58"/>
-      <c r="B21" s="55" t="s">
+      <c r="A21" s="36"/>
+      <c r="B21" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1">
-      <c r="A22" s="58"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
@@ -2083,7 +2541,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A23" s="59"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
@@ -2092,7 +2550,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1">
-      <c r="A24" s="57">
+      <c r="A24" s="34">
         <v>42059</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -2103,7 +2561,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A25" s="59"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="7" t="s">
         <v>7</v>
       </c>
@@ -2135,153 +2593,398 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A1" s="42"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="46">
+      <c r="D2" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="23">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="47" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="23">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="47" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="47" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="23">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="64"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="47" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="23">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="67"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="49" t="s">
+      <c r="A9" s="44"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="67"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="49" t="s">
+      <c r="A10" s="44"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="67"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="49" t="s">
+      <c r="A11" s="44"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="67"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="49" t="s">
+      <c r="A12" s="44"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A13" s="68"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="51" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="52">
+      <c r="D13" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickTop="1"/>
+    <row r="18" spans="1:4" ht="3" customHeight="1" thickBot="1"/>
+    <row r="19" spans="1:4" hidden="1"/>
+    <row r="20" spans="1:4" hidden="1"/>
+    <row r="21" spans="1:4" ht="88.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A21" s="51"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" thickTop="1">
+      <c r="A22" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="65"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="68"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75">
+      <c r="A25" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="71"/>
+      <c r="C25" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="58"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="73"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75">
+      <c r="A29" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="78"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="78"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="78"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="78"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="80"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="88"/>
+      <c r="B35" s="89" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="92"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="92"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="91">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="92"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="90" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="91">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="92"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="94"/>
+      <c r="B40" s="95"/>
+      <c r="C40" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="82"/>
+      <c r="B41" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="86"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A43" s="96"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:B7"/>

</xml_diff>